<commit_message>
First version of eaglecad schematic
</commit_message>
<xml_diff>
--- a/Bill of Material.xlsx
+++ b/Bill of Material.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zach Stamler\Documents\PSU\^ECE411\Practicum\Speedometer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="465" windowWidth="19425" windowHeight="11025" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="470" windowWidth="19420" windowHeight="11020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Bill Of Material</t>
   </si>
@@ -53,9 +48,6 @@
     <t>Nathaniel</t>
   </si>
   <si>
-    <t>Hall Effect Sensors</t>
-  </si>
-  <si>
     <t>Zach</t>
   </si>
   <si>
@@ -102,13 +94,25 @@
   </si>
   <si>
     <t>Dev MCU breakout board</t>
+  </si>
+  <si>
+    <t>US5881TO-92</t>
+  </si>
+  <si>
+    <t>EPL</t>
+  </si>
+  <si>
+    <t>Working Hall Effect Sensors</t>
+  </si>
+  <si>
+    <t>Not Working Hall Effect Sensors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -223,21 +227,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -254,6 +249,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,367 +533,387 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="24.375" style="10" customWidth="1"/>
-    <col min="2" max="2" width="14.375" style="10" customWidth="1"/>
-    <col min="3" max="4" width="13" style="10" customWidth="1"/>
-    <col min="5" max="5" width="19.375" style="10" customWidth="1"/>
-    <col min="6" max="6" width="49" style="10" customWidth="1"/>
-    <col min="7" max="16384" width="10.625" style="11"/>
+    <col min="1" max="1" width="24.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="7" customWidth="1"/>
+    <col min="3" max="4" width="13" style="7" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="49" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="10.58203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1" thickBot="1">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="4">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4">
+        <v>5</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5">
+        <v>3.1</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>3.95</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="8">
-        <v>6</v>
-      </c>
-      <c r="C3" s="8">
-        <v>3.1</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="8" t="s">
+      <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="8">
+      <c r="F5" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="8">
-        <v>3.95</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="8" t="s">
+      <c r="C6" s="5">
+        <v>5.25</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="5">
+        <v>3.48</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5">
+        <v>3.05</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5">
         <v>9</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="8">
-        <v>1</v>
-      </c>
-      <c r="C5" s="8">
-        <v>5.25</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="8">
-        <v>3.48</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8">
-        <v>3.05</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
+      <c r="D9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="8">
-        <v>9</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="E9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-    </row>
-    <row r="10" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-    </row>
-    <row r="29" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-    </row>
-    <row r="31" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-    </row>
-    <row r="32" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
+    </row>
+    <row r="10" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>

<commit_message>
Added in some parts that we'll need to order soon.
</commit_message>
<xml_diff>
--- a/Bill of Material.xlsx
+++ b/Bill of Material.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>Bill Of Material</t>
   </si>
@@ -106,6 +106,24 @@
   </si>
   <si>
     <t>Not Working Hall Effect Sensors</t>
+  </si>
+  <si>
+    <t>JST-PH 2-Pin SMT Right Angle Connector</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>Need to order</t>
+  </si>
+  <si>
+    <t>Lithium Ion Polymer Battery - 3.7v 1200mAh</t>
+  </si>
+  <si>
+    <t>5-way Tactile Switch</t>
+  </si>
+  <si>
+    <t>Sparkfun</t>
   </si>
 </sst>
 </file>
@@ -227,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -249,6 +267,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -258,9 +279,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,7 +552,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -543,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5"/>
@@ -558,14 +577,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1" thickBot="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
       <c r="A2" s="4" t="s">
@@ -588,7 +607,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="4">
@@ -597,13 +616,13 @@
       <c r="C3" s="4">
         <v>5</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -724,28 +743,58 @@
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="A10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="5">
+        <v>4</v>
+      </c>
+      <c r="C10" s="5">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="F10" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="A11" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="5">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="F11" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="A12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="5">
+        <v>5</v>
+      </c>
+      <c r="C12" s="5">
+        <v>9.75</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="F12" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
       <c r="A13" s="5"/>

</xml_diff>

<commit_message>
Added 5-way tactile switch order.
</commit_message>
<xml_diff>
--- a/Bill of Material.xlsx
+++ b/Bill of Material.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>Bill Of Material</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Sparkfun</t>
+  </si>
+  <si>
+    <t>Six 5-way tactile switches.</t>
   </si>
 </sst>
 </file>
@@ -270,6 +273,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -279,7 +283,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,7 +555,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -562,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5"/>
@@ -577,14 +580,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1" thickBot="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
       <c r="A2" s="4" t="s">
@@ -743,7 +746,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="5">
@@ -761,7 +764,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="5">
@@ -779,21 +782,23 @@
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" s="5">
-        <v>9.75</v>
+        <v>17.440000000000001</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="F12" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" ht="27" customHeight="1">

</xml_diff>

<commit_message>
Ordered 4 Li-po batteries and 5 right-angle JST-PH connectors.
</commit_message>
<xml_diff>
--- a/Bill of Material.xlsx
+++ b/Bill of Material.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zach Stamler\Documents\Speed Demon\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="465" windowWidth="19425" windowHeight="11025" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="470" windowWidth="19420" windowHeight="11020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
   <si>
     <t>Bill Of Material</t>
   </si>
@@ -119,12 +114,6 @@
     <t>Adafruit</t>
   </si>
   <si>
-    <t>Need to order</t>
-  </si>
-  <si>
-    <t>Lithium Ion Polymer Battery - 3.7v 1200mAh</t>
-  </si>
-  <si>
     <t>5-way Tactile Switch</t>
   </si>
   <si>
@@ -144,13 +133,28 @@
   </si>
   <si>
     <t>Includes all non-MCU IC/MOS parts for prototyping AND project</t>
+  </si>
+  <si>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>mixec</t>
+  </si>
+  <si>
+    <t>Batteries and connectors from Adafruit</t>
+  </si>
+  <si>
+    <t>Lithium Ion Polymer Battery - 3.7v 2000mAh</t>
+  </si>
+  <si>
+    <t>Battery connector which mounts on the PCB.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -287,6 +291,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -295,27 +320,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -589,42 +593,42 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="48.625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="14.375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="48.58203125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="6" customWidth="1"/>
     <col min="3" max="4" width="13" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="72.625" style="18" customWidth="1"/>
-    <col min="7" max="16384" width="10.625" style="7"/>
+    <col min="5" max="5" width="19.33203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="72.58203125" style="15" customWidth="1"/>
+    <col min="7" max="16384" width="10.58203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -639,12 +643,12 @@
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A3" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="3">
@@ -659,12 +663,12 @@
       <c r="E3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4">
@@ -677,12 +681,12 @@
       <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A5" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="4">
@@ -697,12 +701,12 @@
       <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A6" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="4">
@@ -717,12 +721,12 @@
       <c r="E6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+    <row r="7" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -737,12 +741,12 @@
       <c r="E7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A8" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="4"/>
@@ -755,12 +759,12 @@
       <c r="E8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A9" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="4">
@@ -775,253 +779,251 @@
       <c r="E9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="4">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4">
+        <v>17.440000000000001</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A11" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="4">
+        <v>45.16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="4">
+        <v>9.15</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="4">
+        <v>4</v>
+      </c>
+      <c r="C14" s="4">
+        <v>50</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A15" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="4">
-        <v>4</v>
-      </c>
-      <c r="C10" s="4">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="B15" s="4">
+        <v>5</v>
+      </c>
+      <c r="C15" s="4">
+        <v>3.75</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="4">
-        <v>4</v>
-      </c>
-      <c r="C11" s="4">
-        <v>39.799999999999997</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="4">
-        <v>6</v>
-      </c>
-      <c r="C12" s="4">
-        <v>17.440000000000001</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="4">
-        <v>45.16</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="14"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="14"/>
+      <c r="F15" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A16" s="11"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="14"/>
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A17" s="11"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="14"/>
-    </row>
-    <row r="18" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="14"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A18" s="11"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="14"/>
-    </row>
-    <row r="19" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="14"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A19" s="11"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="14"/>
-    </row>
-    <row r="20" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="14"/>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A20" s="11"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="14"/>
-    </row>
-    <row r="21" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="14"/>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A21" s="11"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="14"/>
-    </row>
-    <row r="22" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="14"/>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A22" s="11"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="14"/>
-    </row>
-    <row r="23" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="14"/>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A23" s="11"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="14"/>
-    </row>
-    <row r="24" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="14"/>
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A24" s="11"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="14"/>
-    </row>
-    <row r="25" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="14"/>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A25" s="11"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="14"/>
-    </row>
-    <row r="26" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="14"/>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A26" s="11"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="14"/>
-    </row>
-    <row r="27" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="14"/>
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A27" s="11"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="14"/>
-    </row>
-    <row r="28" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="14"/>
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A28" s="11"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="14"/>
-    </row>
-    <row r="29" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="14"/>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A29" s="11"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
-      <c r="F29" s="14"/>
-    </row>
-    <row r="30" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="14"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A30" s="11"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
-      <c r="F30" s="14"/>
-    </row>
-    <row r="31" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A31" s="14"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
       <c r="F31" s="14"/>
-    </row>
-    <row r="32" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="14"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="14"/>
-    </row>
-    <row r="33" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="17"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="17"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>

<commit_message>
Added files for OSH stencil. Updated BOM, including total cost per team member.
</commit_message>
<xml_diff>
--- a/Bill of Material.xlsx
+++ b/Bill of Material.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Felix/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Steel Bridge/Users/metalmachine/Speed Demon/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="460" windowWidth="24520" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="51120" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
   <si>
     <t>Bill Of Material</t>
   </si>
@@ -177,6 +177,42 @@
   </si>
   <si>
     <t>Programmer for MCU</t>
+  </si>
+  <si>
+    <t>Main PCB</t>
+  </si>
+  <si>
+    <t>OSH Park</t>
+  </si>
+  <si>
+    <t>Remainder of HW components</t>
+  </si>
+  <si>
+    <t>Shipping incl</t>
+  </si>
+  <si>
+    <t>Solder stencil + solder paste</t>
+  </si>
+  <si>
+    <t>1 ea</t>
+  </si>
+  <si>
+    <t>OSH Stencils</t>
+  </si>
+  <si>
+    <t>Shipping Incl</t>
+  </si>
+  <si>
+    <t>TOTAL PER TEAM MEMBER</t>
+  </si>
+  <si>
+    <t>Remainder of connectors</t>
+  </si>
+  <si>
+    <t>Redco</t>
+  </si>
+  <si>
+    <t>shipping incl</t>
   </si>
 </sst>
 </file>
@@ -228,7 +264,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -301,11 +337,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -343,6 +409,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -352,6 +420,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,33 +701,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48.6640625" style="12" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" style="5" customWidth="1"/>
-    <col min="3" max="4" width="13" style="5" customWidth="1"/>
+    <col min="3" max="3" width="13" style="5" customWidth="1"/>
+    <col min="4" max="4" width="16" style="5" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" style="5" customWidth="1"/>
     <col min="6" max="6" width="72.6640625" style="12" customWidth="1"/>
-    <col min="7" max="16384" width="10.6640625" style="6"/>
+    <col min="7" max="7" width="10.6640625" style="6"/>
+    <col min="8" max="8" width="31.33203125" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="10.6640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="17"/>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19"/>
+      <c r="H1" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="20"/>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -677,8 +753,12 @@
       <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="16">
+        <f>SUM(C2:C100)/4</f>
+        <v>105.95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>24</v>
       </c>
@@ -698,7 +778,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
@@ -716,7 +796,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
@@ -736,7 +816,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>14</v>
       </c>
@@ -756,7 +836,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
@@ -776,7 +856,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>18</v>
       </c>
@@ -794,7 +874,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>21</v>
       </c>
@@ -814,7 +894,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>28</v>
       </c>
@@ -832,7 +912,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>31</v>
       </c>
@@ -850,7 +930,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>32</v>
       </c>
@@ -870,7 +950,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>35</v>
       </c>
@@ -890,7 +970,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>18</v>
       </c>
@@ -906,7 +986,7 @@
       </c>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>39</v>
       </c>
@@ -924,7 +1004,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>41</v>
       </c>
@@ -997,36 +1077,78 @@
       </c>
     </row>
     <row r="20" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="A20" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="3">
+        <v>4</v>
+      </c>
+      <c r="C20" s="3">
+        <v>27.75</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="9"/>
+    <row r="21" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="9"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="9"/>
-    </row>
-    <row r="23" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="9"/>
+      <c r="C21" s="3">
+        <v>95</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="3">
+        <v>47.49</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>59</v>
+      </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="9"/>
+      <c r="C23" s="3">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="24" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>

</xml_diff>

<commit_message>
Updated some of my orders
</commit_message>
<xml_diff>
--- a/Bill of Material.xlsx
+++ b/Bill of Material.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Steel Bridge/Users/metalmachine/Speed Demon/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="51120" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="19420" windowHeight="11020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
   <si>
     <t>Bill Of Material</t>
   </si>
@@ -50,9 +45,6 @@
     <t>A3212EUA-T</t>
   </si>
   <si>
-    <t>Nathaniel</t>
-  </si>
-  <si>
     <t>Zach</t>
   </si>
   <si>
@@ -119,9 +111,6 @@
     <t>Adafruit</t>
   </si>
   <si>
-    <t>Need to order</t>
-  </si>
-  <si>
     <t>Lithium Ion Polymer Battery - 3.7v 1200mAh</t>
   </si>
   <si>
@@ -213,13 +202,28 @@
   </si>
   <si>
     <t>shipping incl</t>
+  </si>
+  <si>
+    <t>Nathan</t>
+  </si>
+  <si>
+    <t>Six JST-PH connectors</t>
+  </si>
+  <si>
+    <t>Four Li-Po batteries</t>
+  </si>
+  <si>
+    <t>Female/Female Jumper wires 40x3"</t>
+  </si>
+  <si>
+    <t>Two sets of 40 female/female jumper wires. Half of shipping cost included. The other half goes toward Linyi's personal order</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -411,6 +415,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -420,7 +425,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,21 +697,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="48.6640625" style="12" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" style="5" customWidth="1"/>
@@ -720,21 +724,21 @@
     <col min="9" max="16384" width="10.6640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="20"/>
       <c r="H1" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" s="20"/>
-    </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="J1" s="17"/>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -745,7 +749,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>4</v>
@@ -755,12 +759,12 @@
       </c>
       <c r="H2" s="16">
         <f>SUM(C2:C100)/4</f>
-        <v>105.95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>108.45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1">
         <v>5</v>
@@ -769,16 +773,16 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
@@ -790,15 +794,15 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -807,18 +811,18 @@
         <v>3.95</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A6" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -827,56 +831,56 @@
         <v>5.25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C7" s="1">
         <v>3.48</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A8" s="10" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>18</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1">
         <v>3.05</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="10" t="s">
+    </row>
+    <row r="9" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A9" s="10" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>21</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -885,18 +889,18 @@
         <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A10" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1">
         <v>4</v>
@@ -905,16 +909,18 @@
         <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A11" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>31</v>
       </c>
       <c r="B11" s="1">
         <v>4</v>
@@ -923,16 +929,18 @@
         <v>39.799999999999997</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="F11" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A12" s="10" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>32</v>
       </c>
       <c r="B12" s="1">
         <v>6</v>
@@ -941,54 +949,54 @@
         <v>17.440000000000001</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="10" t="s">
+      <c r="B13" s="1" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="C13" s="1">
         <v>45.16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1">
         <v>7.5</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A15" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -998,15 +1006,15 @@
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A16" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -1016,15 +1024,15 @@
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A17" s="13" t="s">
         <v>40</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>42</v>
       </c>
       <c r="B17" s="14">
         <v>3</v>
@@ -1034,15 +1042,15 @@
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A18" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" s="14">
         <v>1</v>
@@ -1052,15 +1060,15 @@
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A19" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="14">
         <v>1</v>
@@ -1070,15 +1078,15 @@
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A20" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20" s="3">
         <v>4</v>
@@ -1087,78 +1095,90 @@
         <v>27.75</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3">
         <v>95</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A22" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="C22" s="3">
         <v>47.49</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A23" s="10" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>59</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3">
         <v>32.700000000000003</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
+      <c r="A24" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="3">
+        <v>2</v>
+      </c>
+      <c r="C24" s="3">
+        <v>10</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="9"/>
-    </row>
-    <row r="25" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A25" s="9"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1166,7 +1186,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A26" s="9"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1174,7 +1194,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A27" s="9"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1182,7 +1202,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A28" s="9"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1190,7 +1210,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="9"/>
     </row>
-    <row r="29" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A29" s="9"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1198,7 +1218,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="9"/>
     </row>
-    <row r="30" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A30" s="9"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1206,7 +1226,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="9"/>
     </row>
-    <row r="31" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A31" s="9"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1214,7 +1234,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="9"/>
     </row>
-    <row r="32" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A32" s="9"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1222,7 +1242,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="9"/>
     </row>
-    <row r="33" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" s="2" customFormat="1" ht="27" customHeight="1">
       <c r="A33" s="11"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>

</xml_diff>